<commit_message>
Updated IYCF in costs and coverage tab
</commit_message>
<xml_diff>
--- a/Projects/Tanzania/data/regional/InputForCode_Arusha.xlsx
+++ b/Projects/Tanzania/data/regional/InputForCode_Arusha.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Nutrition\applications\tanzania\data\regional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\Nutrition\Projects\Tanzania\data\regional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19260" windowHeight="15540" tabRatio="500" firstSheet="26" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19260" windowHeight="15540" tabRatio="500" firstSheet="26" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="50" r:id="rId1"/>
@@ -14775,11 +14775,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14790,6 +14785,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -25234,8 +25234,8 @@
   <sheetPr codeName="Sheet29"/>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25927,7 +25927,7 @@
         <v>157</v>
       </c>
       <c r="B49" s="127">
-        <v>0.107</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="C49" s="145">
         <v>0.95</v>
@@ -26597,7 +26597,7 @@
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>

</xml_diff>